<commit_message>
Updated for Rapise 5.6
</commit_message>
<xml_diff>
--- a/CreatePurchaseOrder/CreatePurchaseOrder.rvl.xlsx
+++ b/CreatePurchaseOrder/CreatePurchaseOrder.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="173">
   <si>
     <t>Flow</t>
   </si>
@@ -523,6 +523,15 @@
   </si>
   <si>
     <t>rowCount</t>
+  </si>
+  <si>
+    <t>Navigator</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>url</t>
   </si>
 </sst>
 </file>
@@ -543,7 +552,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="177">
+  <borders count="178">
     <border>
       <left/>
       <right/>
@@ -727,11 +736,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
@@ -909,6 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="174" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="175" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="176" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="177" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -961,6 +972,18 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -1533,7 +1556,7 @@
         <v>20</v>
       </c>
       <c r="G39" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40">
@@ -1884,7 +1907,7 @@
         <v>20</v>
       </c>
       <c r="G63" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="64">

</xml_diff>

<commit_message>
Collapse header before entering lines
</commit_message>
<xml_diff>
--- a/CreatePurchaseOrder/CreatePurchaseOrder.rvl.xlsx
+++ b/CreatePurchaseOrder/CreatePurchaseOrder.rvl.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="175">
   <si>
     <t>Flow</t>
   </si>
@@ -532,6 +532,12 @@
   </si>
   <si>
     <t>url</t>
+  </si>
+  <si>
+    <t>purchtablelistpage_LineViewTab1</t>
+  </si>
+  <si>
+    <t>Purchase order header</t>
   </si>
 </sst>
 </file>
@@ -1285,6 +1291,24 @@
       <c r="A21" t="s">
         <v>7</v>
       </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">

</xml_diff>